<commit_message>
tested e2e first feature
</commit_message>
<xml_diff>
--- a/src/assets/e2e-document.xlsx
+++ b/src/assets/e2e-document.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbt\dev\HighLike\src\assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbt\dev2\HighLike\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12240"/>
   </bookViews>
   <sheets>
     <sheet name="איתור מועמדים לפי עיר מגורים" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>תרחיש בדיקה</t>
   </si>
@@ -109,12 +109,22 @@
   <si>
     <t>קבלת כלל האנשים שקיימים במאגר שיש להם שנות ניסיון לפי מה ההוגדר בחיפוש, יש לשים לב שעל שנת נסיון 1 לא יחזור 10 שנות נסיון</t>
   </si>
+  <si>
+    <t>הוזן 'תל אביב', התוצאה 
+של חולון לא חזרה והתקבלו תוצאות מתל אביב בלבד כנדרש</t>
+  </si>
+  <si>
+    <t>הוזן 'חולון', התקלה תוצאה 1 כנדרש</t>
+  </si>
+  <si>
+    <t>מחזיר את כלל התוצאות במאגר כנדרש</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,8 +155,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -156,6 +173,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -183,11 +205,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -198,10 +221,14 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="חישוב" xfId="1" builtinId="22"/>
+    <cellStyle name="טוב" xfId="2" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -515,65 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView rightToLeft="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="26" style="1" customWidth="1"/>
-    <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="63.140625" style="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:3" ht="42" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="2"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
-  <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,6 +566,71 @@
     </row>
     <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView rightToLeft="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="A2:C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26" style="1" customWidth="1"/>
+    <col min="2" max="2" width="57.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="63.140625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="42" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="2" t="s">

</xml_diff>